<commit_message>
cleared code, submission part added
</commit_message>
<xml_diff>
--- a/Workbook.xlsx
+++ b/Workbook.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandredumur/Documents/EPFL/MA/MA1/ML/ML_project2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\GitHub\ML_project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="460" windowWidth="24380" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="1220" yWindow="460" windowWidth="24380" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,20 +27,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Methode</t>
-  </si>
-  <si>
-    <t>Model</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="23">
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>linear classifier</t>
+  </si>
+  <si>
+    <t>pertinence</t>
+  </si>
+  <si>
+    <t>GloVe</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>nb_iters</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>0.996</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>53.125</t>
+  </si>
+  <si>
+    <t>50.5</t>
+  </si>
+  <si>
+    <t>neural network</t>
+  </si>
+  <si>
+    <t>62.125</t>
+  </si>
+  <si>
+    <t>60.125</t>
+  </si>
+  <si>
+    <t>62.375</t>
+  </si>
+  <si>
+    <t>63.25</t>
+  </si>
+  <si>
+    <t>61.0</t>
+  </si>
+  <si>
+    <t>lower bound on somme</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>61.125</t>
+  </si>
+  <si>
+    <t>61.625</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>68.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -68,8 +139,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -79,6 +152,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -346,24 +422,321 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C5:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="23.9140625" customWidth="1"/>
+    <col min="8" max="8" width="20.75" customWidth="1"/>
+    <col min="9" max="9" width="21.4140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
         <v>1</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2">
+        <v>80000</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2">
+        <v>40000</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2">
+        <v>4000</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>2000</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17">
+        <v>50</v>
+      </c>
+      <c r="I17" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Vocab augmented (author = Alex)
</commit_message>
<xml_diff>
--- a/Workbook.xlsx
+++ b/Workbook.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="26">
   <si>
     <t>model</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>68.5</t>
+  </si>
+  <si>
+    <t>GloVe used</t>
+  </si>
+  <si>
+    <t>their</t>
+  </si>
+  <si>
+    <t>ours</t>
   </si>
 </sst>
 </file>
@@ -423,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C5:I17"/>
+  <dimension ref="C5:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -436,7 +445,7 @@
     <col min="9" max="9" width="21.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,8 +467,11 @@
       <c r="I5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="J5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -481,8 +493,11 @@
       <c r="I6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>1</v>
       </c>
@@ -504,8 +519,11 @@
       <c r="I7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="J7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>1</v>
       </c>
@@ -527,8 +545,11 @@
       <c r="I8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>11</v>
       </c>
@@ -550,8 +571,11 @@
       <c r="I9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="J9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>11</v>
       </c>
@@ -573,8 +597,11 @@
       <c r="I10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>11</v>
       </c>
@@ -596,8 +623,11 @@
       <c r="I11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="J11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>11</v>
       </c>
@@ -619,8 +649,11 @@
       <c r="I12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="J12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>11</v>
       </c>
@@ -642,8 +675,11 @@
       <c r="I13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="J13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>11</v>
       </c>
@@ -665,8 +701,11 @@
       <c r="I14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="J14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>11</v>
       </c>
@@ -688,8 +727,11 @@
       <c r="I15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="J15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>11</v>
       </c>
@@ -706,33 +748,455 @@
         <v>7</v>
       </c>
       <c r="H16">
+        <v>50</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17">
+        <v>100</v>
+      </c>
+      <c r="I17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18">
+        <v>500</v>
+      </c>
+      <c r="I18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19">
+        <v>35</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <v>1000</v>
+      </c>
+      <c r="I19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>35</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20">
         <v>2000</v>
       </c>
-      <c r="I16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17">
-        <v>35</v>
-      </c>
-      <c r="E17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17">
+      <c r="I20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>35</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21">
+        <v>5000</v>
+      </c>
+      <c r="I21" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22">
+        <v>10000</v>
+      </c>
+      <c r="I22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23">
+        <v>20000</v>
+      </c>
+      <c r="I23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24">
+        <v>50000</v>
+      </c>
+      <c r="I24" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25">
+        <v>35</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25">
         <v>50</v>
       </c>
-      <c r="I17" t="s">
-        <v>21</v>
+      <c r="I25" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>35</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26">
+        <v>100</v>
+      </c>
+      <c r="I26" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>35</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27">
+        <v>500</v>
+      </c>
+      <c r="I27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>35</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28">
+        <v>1000</v>
+      </c>
+      <c r="I28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>35</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29">
+        <v>2000</v>
+      </c>
+      <c r="I29" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <v>35</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30">
+        <v>5000</v>
+      </c>
+      <c r="I30" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31">
+        <v>10000</v>
+      </c>
+      <c r="I31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32">
+        <v>35</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32">
+        <v>20000</v>
+      </c>
+      <c r="I32" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33">
+        <v>35</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33">
+        <v>50000</v>
+      </c>
+      <c r="I33" t="s">
+        <v>22</v>
+      </c>
+      <c r="J33" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>